<commit_message>
doc file am thanh
</commit_message>
<xml_diff>
--- a/PBL5_Final/file2.xlsx
+++ b/PBL5_Final/file2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PBL5_Final\PBL5_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A824C45-D661-4150-B65E-73EAF1052483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056B02EF-A9BC-4548-A1FE-7622372AC19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C092ADE7-E2F3-4EBC-85B2-A3AF89B0D8F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>A</t>
   </si>
@@ -85,6 +85,111 @@
   <si>
     <t>もんだい1 の ことばは ひらがなで どう かきますか。1・2・3・4から いちばん いい ものを ひとつ えらんで
 ください。</t>
+  </si>
+  <si>
+    <t>いそがしかった</t>
+  </si>
+  <si>
+    <t>すずしかった</t>
+  </si>
+  <si>
+    <t>たのしかった</t>
+  </si>
+  <si>
+    <t>かなしかった</t>
+  </si>
+  <si>
+    <t>かたち</t>
+  </si>
+  <si>
+    <t>いろ</t>
+  </si>
+  <si>
+    <t>におい</t>
+  </si>
+  <si>
+    <t>あじ</t>
+  </si>
+  <si>
+    <t>ふべん</t>
+  </si>
+  <si>
+    <t>ぶべん</t>
+  </si>
+  <si>
+    <t>ふへん</t>
+  </si>
+  <si>
+    <t>ぶへん</t>
+  </si>
+  <si>
+    <t>もんだい2 の ことばは どう かきますか。1・2・3・4からいちばん いい ものを ひとつ えらんで ください。</t>
+  </si>
+  <si>
+    <t>白い</t>
+  </si>
+  <si>
+    <t>黒い</t>
+  </si>
+  <si>
+    <t>赤い</t>
+  </si>
+  <si>
+    <t>青い</t>
+  </si>
+  <si>
+    <t>計書</t>
+  </si>
+  <si>
+    <t>訂画</t>
+  </si>
+  <si>
+    <t>計画</t>
+  </si>
+  <si>
+    <t>訂書</t>
+  </si>
+  <si>
+    <t>言語知識(文法)</t>
+  </si>
+  <si>
+    <t>もんだい1 ( )に 何を 入れますか。1・2・3・4から いちばんいい ものを 一つ えらんで ください。</t>
+  </si>
+  <si>
+    <t>きのうの しゅくだいは 少なかったので、( ) 終わりました。</t>
+  </si>
+  <si>
+    <t>20 分</t>
+  </si>
+  <si>
+    <t>20 分しか</t>
+  </si>
+  <si>
+    <t>20 分で</t>
+  </si>
+  <si>
+    <t>20 分を</t>
+  </si>
+  <si>
+    <t>もんだい2 ★ に 入る ものは どれですか。1・2・3・4から いちばんいい ものを 一つ えらんで ください。</t>
+  </si>
+  <si>
+    <t>先月まで 花屋が あった ____       ___★__        ____       ____ おいしいです。</t>
+  </si>
+  <si>
+    <t>できた</t>
+  </si>
+  <si>
+    <t>りんごの ケーキが</t>
+  </si>
+  <si>
+    <t>きっさてんは</t>
+  </si>
+  <si>
+    <t>場所に</t>
+  </si>
+  <si>
+    <t>D:\PBL5_Final\PBL5_Final\media\media\5.png</t>
   </si>
   <si>
     <r>
@@ -94,7 +199,7 @@
       <rPr>
         <u/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -105,7 +210,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -114,18 +219,6 @@
     </r>
   </si>
   <si>
-    <t>いそがしかった</t>
-  </si>
-  <si>
-    <t>すずしかった</t>
-  </si>
-  <si>
-    <t>たのしかった</t>
-  </si>
-  <si>
-    <t>かなしかった</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">わたしは この </t>
     </r>
@@ -133,7 +226,7 @@
       <rPr>
         <u/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -144,7 +237,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -153,18 +246,6 @@
     </r>
   </si>
   <si>
-    <t>かたち</t>
-  </si>
-  <si>
-    <t>いろ</t>
-  </si>
-  <si>
-    <t>におい</t>
-  </si>
-  <si>
-    <t>あじ</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">この あたりは ちょっと </t>
     </r>
@@ -172,7 +253,7 @@
       <rPr>
         <u/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -183,7 +264,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -192,38 +273,45 @@
     </r>
   </si>
   <si>
-    <t>ふべん</t>
-  </si>
-  <si>
-    <t>ぶべん</t>
-  </si>
-  <si>
-    <t>ふへん</t>
-  </si>
-  <si>
-    <t>ぶへん</t>
-  </si>
-  <si>
-    <t>もんだい2 の ことばは どう かきますか。1・2・3・4からいちばん いい ものを ひとつ えらんで ください。</t>
-  </si>
-  <si>
-    <t>白い</t>
-  </si>
-  <si>
-    <t>黒い</t>
-  </si>
-  <si>
-    <t>赤い</t>
-  </si>
-  <si>
-    <t>青い</t>
-  </si>
-  <si>
+    <r>
+      <t>なつやすみの</t>
+    </r>
     <r>
       <rPr>
         <u/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> けいかく</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>は まだ きまって いません。</t>
+    </r>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>D:\PBL5_Final\PBL5_Final\media\media\02.Track02.mp3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -233,99 +321,33 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> くつしたが ほしいです。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>なつやすみの</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> けいかく</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>は まだ きまって いません。</t>
-    </r>
-  </si>
-  <si>
-    <t>計書</t>
-  </si>
-  <si>
-    <t>訂画</t>
-  </si>
-  <si>
-    <t>計画</t>
-  </si>
-  <si>
-    <t>訂書</t>
-  </si>
-  <si>
-    <t>言語知識(文法)</t>
-  </si>
-  <si>
-    <t>もんだい1 ( )に 何を 入れますか。1・2・3・4から いちばんいい ものを 一つ えらんで ください。</t>
-  </si>
-  <si>
-    <t>きのうの しゅくだいは 少なかったので、( ) 終わりました。</t>
-  </si>
-  <si>
-    <t>20 分</t>
-  </si>
-  <si>
-    <t>20 分しか</t>
-  </si>
-  <si>
-    <t>20 分で</t>
-  </si>
-  <si>
-    <t>20 分を</t>
-  </si>
-  <si>
-    <t>もんだい2 ★ に 入る ものは どれですか。1・2・3・4から いちばんいい ものを 一つ えらんで ください。</t>
-  </si>
-  <si>
-    <t>先月まで 花屋が あった ____       ___★__        ____       ____ おいしいです。</t>
-  </si>
-  <si>
-    <t>できた</t>
-  </si>
-  <si>
-    <t>りんごの ケーキが</t>
-  </si>
-  <si>
-    <t>きっさてんは</t>
-  </si>
-  <si>
-    <t>場所に</t>
+      <t>くつしたが ほしいです。</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,7 +362,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -350,7 +371,34 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -377,12 +425,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF1AB35-4D71-4E38-B7DC-3DCE46F44D1C}">
-  <dimension ref="E1:O8"/>
+  <dimension ref="B1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -720,7 +771,7 @@
     <col min="13" max="13" width="12.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>4</v>
       </c>
@@ -734,28 +785,34 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="5:15" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
       <c r="E2" t="s">
         <v>14</v>
       </c>
@@ -768,29 +825,32 @@
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2">
+      <c r="O2" s="3">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="5:15" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" t="s">
         <v>14</v>
       </c>
@@ -803,29 +863,32 @@
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3">
+      <c r="O3" s="3">
         <v>10</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="5:15" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
       <c r="E4" t="s">
         <v>14</v>
       </c>
@@ -838,29 +901,32 @@
       <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4">
+      <c r="O4" s="3">
         <v>10</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="5:15" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
       <c r="E5" t="s">
         <v>14</v>
       </c>
@@ -871,31 +937,35 @@
         <v>123</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="N5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5">
+      <c r="O5" s="3">
         <v>10</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="5:15" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" t="s">
         <v>14</v>
       </c>
@@ -906,33 +976,39 @@
         <v>123</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="3">
+        <v>10</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" t="s">
         <v>37</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="O6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="5:15" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>42</v>
       </c>
       <c r="F7">
         <v>20</v>
@@ -941,33 +1017,39 @@
         <v>1234</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7">
+      <c r="O7" s="3">
         <v>10</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="5:15" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>20</v>
@@ -976,30 +1058,77 @@
         <v>1234</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
         <v>50</v>
       </c>
-      <c r="J8" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8">
+      <c r="J8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="3">
         <v>10</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="2:16" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>1234</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="3">
+        <v>10</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>